<commit_message>
attach doc, select keywords added
</commit_message>
<xml_diff>
--- a/TestData/WKD_TESTDATA_IMPL2.xlsx
+++ b/TestData/WKD_TESTDATA_IMPL2.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beimnet.bekele\Documents\Enviroments\robot-third\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEE4C6C-AF3B-4E7D-BD41-DD1BE1AB5BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D76AB2-3854-42A2-BB3A-0D5C727588A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change_SIM" sheetId="6" r:id="rId1"/>
-    <sheet name="TestData_ServiceID2" sheetId="65" state="hidden" r:id="rId2"/>
+    <sheet name="ADJUST_ACCOUNT" sheetId="67" r:id="rId2"/>
+    <sheet name="TestData_ServiceID2" sheetId="65" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -334,7 +335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="151">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -740,12 +741,60 @@
   <si>
     <t>251799135309</t>
   </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>TC_002</t>
+  </si>
+  <si>
+    <t>Increment</t>
+  </si>
+  <si>
+    <t>Decrement</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Adjust Main Account Prepaid</t>
+  </si>
+  <si>
+    <t>Adjust Account Increment</t>
+  </si>
+  <si>
+    <t>Add air time</t>
+  </si>
+  <si>
+    <t>251700408785</t>
+  </si>
+  <si>
+    <t>Somefile</t>
+  </si>
+  <si>
+    <t>1400</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>ChangeS</t>
+  </si>
+  <si>
+    <t>Adjust Account Increment-EBU</t>
+  </si>
+  <si>
+    <t>Adjust Main Account Prepaid_EBU</t>
+  </si>
+  <si>
+    <t>251700404232</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -823,6 +872,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -922,7 +977,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -982,6 +1037,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1261,8 +1320,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:DJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1556,6 +1615,384 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D582692-9D11-41A5-A3F7-28932A5CB46C}">
+  <dimension ref="A1:DJ4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="61.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:114" s="14" customFormat="1">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
+      <c r="W1"/>
+      <c r="X1"/>
+      <c r="Y1"/>
+      <c r="Z1"/>
+      <c r="AA1"/>
+      <c r="AB1"/>
+      <c r="AC1"/>
+      <c r="AD1"/>
+      <c r="AE1"/>
+      <c r="AF1"/>
+      <c r="AG1"/>
+      <c r="AH1"/>
+      <c r="AI1"/>
+      <c r="AJ1"/>
+      <c r="AK1"/>
+      <c r="AL1"/>
+      <c r="AM1"/>
+      <c r="AN1"/>
+      <c r="AO1"/>
+      <c r="AP1"/>
+      <c r="AQ1"/>
+      <c r="AR1"/>
+      <c r="AS1"/>
+      <c r="AT1"/>
+      <c r="AU1"/>
+      <c r="AV1"/>
+      <c r="AW1"/>
+      <c r="AX1"/>
+      <c r="AY1"/>
+      <c r="AZ1"/>
+      <c r="BA1"/>
+      <c r="BB1"/>
+      <c r="BC1"/>
+      <c r="BD1"/>
+      <c r="BE1"/>
+      <c r="BF1"/>
+      <c r="BG1"/>
+      <c r="BH1"/>
+      <c r="BI1"/>
+      <c r="BJ1"/>
+      <c r="BK1"/>
+      <c r="BL1"/>
+      <c r="BM1"/>
+      <c r="BN1"/>
+      <c r="BO1"/>
+      <c r="BP1"/>
+      <c r="BQ1"/>
+      <c r="BR1"/>
+      <c r="BS1"/>
+      <c r="BT1"/>
+      <c r="BU1"/>
+      <c r="BV1"/>
+      <c r="BW1"/>
+      <c r="BX1"/>
+      <c r="BY1"/>
+      <c r="BZ1"/>
+      <c r="CA1"/>
+      <c r="CB1"/>
+      <c r="CC1"/>
+      <c r="CD1"/>
+      <c r="CE1"/>
+      <c r="CF1"/>
+      <c r="CG1"/>
+      <c r="CH1"/>
+      <c r="CI1"/>
+      <c r="CJ1"/>
+      <c r="CK1"/>
+      <c r="CL1"/>
+      <c r="CM1"/>
+      <c r="CN1"/>
+      <c r="CO1"/>
+      <c r="CP1"/>
+      <c r="CQ1"/>
+      <c r="CR1"/>
+      <c r="CS1"/>
+      <c r="CT1"/>
+      <c r="CU1"/>
+      <c r="CV1"/>
+      <c r="CW1"/>
+      <c r="CX1"/>
+      <c r="CY1"/>
+      <c r="CZ1"/>
+      <c r="DA1"/>
+      <c r="DB1"/>
+      <c r="DC1"/>
+      <c r="DD1"/>
+      <c r="DE1"/>
+      <c r="DF1"/>
+      <c r="DG1"/>
+      <c r="DH1"/>
+      <c r="DI1"/>
+      <c r="DJ1"/>
+    </row>
+    <row r="2" spans="1:114" s="13" customFormat="1">
+      <c r="A2" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+      <c r="AO2"/>
+      <c r="AP2"/>
+      <c r="AQ2"/>
+      <c r="AR2"/>
+      <c r="AS2"/>
+      <c r="AT2"/>
+      <c r="AU2"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
+      <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BB2"/>
+      <c r="BC2"/>
+      <c r="BD2"/>
+      <c r="BE2"/>
+      <c r="BF2"/>
+      <c r="BG2"/>
+      <c r="BH2"/>
+      <c r="BI2"/>
+      <c r="BJ2"/>
+      <c r="BK2"/>
+      <c r="BL2"/>
+      <c r="BM2"/>
+      <c r="BN2"/>
+      <c r="BO2"/>
+      <c r="BP2"/>
+      <c r="BQ2"/>
+      <c r="BR2"/>
+      <c r="BS2"/>
+      <c r="BT2"/>
+      <c r="BU2"/>
+      <c r="BV2"/>
+      <c r="BW2"/>
+      <c r="BX2"/>
+      <c r="BY2"/>
+      <c r="BZ2"/>
+      <c r="CA2"/>
+      <c r="CB2"/>
+      <c r="CC2"/>
+      <c r="CD2"/>
+      <c r="CE2"/>
+      <c r="CF2"/>
+      <c r="CG2"/>
+      <c r="CH2"/>
+      <c r="CI2"/>
+      <c r="CJ2"/>
+      <c r="CK2"/>
+      <c r="CL2"/>
+      <c r="CM2"/>
+      <c r="CN2"/>
+      <c r="CO2"/>
+      <c r="CP2"/>
+      <c r="CQ2"/>
+      <c r="CR2"/>
+      <c r="CS2"/>
+      <c r="CT2"/>
+      <c r="CU2"/>
+      <c r="CV2"/>
+      <c r="CW2"/>
+      <c r="CX2"/>
+      <c r="CY2"/>
+      <c r="CZ2"/>
+      <c r="DA2"/>
+      <c r="DB2"/>
+      <c r="DC2"/>
+      <c r="DD2"/>
+      <c r="DE2"/>
+      <c r="DF2"/>
+      <c r="DG2"/>
+      <c r="DH2"/>
+      <c r="DI2"/>
+      <c r="DJ2"/>
+    </row>
+    <row r="3" spans="1:114">
+      <c r="A3" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:114">
+      <c r="A4" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 C2 - Restricted Information</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AO983"/>
   <sheetViews>

</xml_diff>